<commit_message>
Added test case number 5
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testData/Test_Data_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\Selenium_Training_B16\Selenium_Training_B16_MVN\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\sunil_branch\SeleniumTraining_B16_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0812C91E-7EC1-46A8-9600-ABB559E60A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BB3D15-E04B-4E1B-B937-EEF5BD3C785C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="86">
   <si>
     <t>Sr.No</t>
   </si>
@@ -281,6 +281,12 @@
   </si>
   <si>
     <t>1999</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Concept</t>
   </si>
 </sst>
 </file>
@@ -660,11 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,7 +716,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -728,7 +733,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -762,7 +767,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -779,7 +784,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -813,7 +818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -830,7 +835,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -865,13 +870,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E11" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Regression"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{E3D1410E-F577-46E5-AF83-4F9B0549376C}">
@@ -884,10 +883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1429,6 +1428,93 @@
         <v>28</v>
       </c>
     </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1437,6 +1523,7 @@
     <hyperlink ref="C11" r:id="rId3" xr:uid="{7226DC3E-DCFF-45E7-A0C1-E55C7D84654F}"/>
     <hyperlink ref="C15" r:id="rId4" xr:uid="{7DB34973-6C7C-4368-8A8E-A565BB13F4BA}"/>
     <hyperlink ref="C23" r:id="rId5" xr:uid="{35559D0A-FE78-4859-AEF3-78E38A24F8F0}"/>
+    <hyperlink ref="C27" r:id="rId6" xr:uid="{5279187B-7E2F-4201-86A4-EA21FCDA1DAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
executimng 2 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testData/Test_Data_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\Selenium_Training_B16\Selenium_Training_B16_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24E443D-7E24-43EB-9CE0-C53A007222AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D72812B-2CB5-4D96-A977-BA6AD684F102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="2" r:id="rId1"/>
@@ -670,7 +670,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,7 +751,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -759,7 +759,7 @@
         <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>49</v>
@@ -853,7 +853,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -861,7 +861,7 @@
         <v>58</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>49</v>

</xml_diff>